<commit_message>
preenchimento de fornecedor e remessa
</commit_message>
<xml_diff>
--- a/base teste.xlsx
+++ b/base teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salomao\Desktop\codigos\controle\projeto_pedidos_cimed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256C7FCD-10DB-438C-8CAF-3F2AE47555BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0816EA4E-5923-4820-AF5E-40774DEB5C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D85B9F9A-EC1B-4E84-84D3-F9421CEEDFCD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Pedido</t>
   </si>
@@ -48,6 +48,45 @@
   </si>
   <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Sabonete</t>
+  </si>
+  <si>
+    <t>Detergente</t>
+  </si>
+  <si>
+    <t>Acido tipo 2</t>
+  </si>
+  <si>
+    <t>Etanol</t>
+  </si>
+  <si>
+    <t>Acido TIpo 1</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Data de Remessa</t>
+  </si>
+  <si>
+    <t>Fornecedor</t>
+  </si>
+  <si>
+    <t>Follow-up</t>
+  </si>
+  <si>
+    <t>Merck</t>
+  </si>
+  <si>
+    <t>Aguardando importação</t>
+  </si>
+  <si>
+    <t>Fora de estoque</t>
   </si>
 </sst>
 </file>
@@ -83,8 +122,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,83 +459,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF12401-A4FE-4E23-8584-A74D3CA84811}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(RIGHT(B2,5),C2)</f>
+        <v>7319910</v>
+      </c>
+      <c r="B2">
         <v>4600073199</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
+      <c r="F2" s="1">
+        <v>45667</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A6" si="0">_xlfn.CONCAT(RIGHT(B3,5),C3)</f>
+        <v>7319920</v>
+      </c>
+      <c r="B3">
         <v>4600073199</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="1">
+        <v>45677</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>7319930</v>
+      </c>
+      <c r="B4">
         <v>4600073199</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>2</v>
       </c>
+      <c r="F4" s="1">
+        <v>45669</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>7319940</v>
+      </c>
+      <c r="B5">
         <v>4600073199</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>2</v>
       </c>
+      <c r="F5" s="1">
+        <v>45677</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>7319950</v>
+      </c>
+      <c r="B6">
         <v>4600073199</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45677</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>